<commit_message>
Start of VAR model
Defining workflow to follow
</commit_message>
<xml_diff>
--- a/italy_values_dataset.xlsx
+++ b/italy_values_dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oldan\Desktop\RURAL DEVELOPMENT\.venv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oldan\Desktop\RuralDevelopment\progetto-tirocinio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF754AF-18E9-4C26-B2CB-427FC769AD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686DB74A-80C8-4582-BE44-856648857A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,15 +240,6 @@
     <t>Rural population</t>
   </si>
   <si>
-    <t>Employment in agriculture (% of total employment) (modeled ILO estimate)</t>
-  </si>
-  <si>
-    <t>Employment in agriculture, male (% of male employment) (modeled ILO estimate)</t>
-  </si>
-  <si>
-    <t>Employment in agriculture, female (% of female employment) (modeled ILO estimate)</t>
-  </si>
-  <si>
     <t>Agriculture, forestry, and fishing, value added (% of GDP)</t>
   </si>
   <si>
@@ -331,6 +322,15 @@
   </si>
   <si>
     <t>Fertilizer consumption (% of fertilizer production)</t>
+  </si>
+  <si>
+    <t>Employment in agriculture, female (% of female employment)</t>
+  </si>
+  <si>
+    <t>Employment in agriculture, male (% of male employment)</t>
+  </si>
+  <si>
+    <t>Employment in agriculture (% of total employment)</t>
   </si>
 </sst>
 </file>
@@ -786,7 +786,7 @@
   <dimension ref="A1:BN37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AF5">
         <v>1.2353375560173501</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="AF6">
         <v>100</v>
@@ -1714,7 +1714,7 @@
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="AG7">
         <v>8.4428416366504102</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="8" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="AG8">
         <v>8.2631918038944097</v>
@@ -1922,7 +1922,7 @@
     </row>
     <row r="9" spans="1:66" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="AG9">
         <v>8.7868252349311202</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="10" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C10">
         <v>301340</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="11" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C11">
         <v>294110</v>
@@ -2408,7 +2408,7 @@
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AF12">
         <v>279865.12052792002</v>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="AF13">
         <v>2.9656347117507602</v>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AF14">
         <v>8837.2148127599994</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AF15">
         <v>25.805820951344732</v>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="AF16">
         <v>75897.5</v>
@@ -2658,7 +2658,7 @@
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C17">
         <v>70.324028424739041</v>
@@ -2849,7 +2849,7 @@
     </row>
     <row r="18" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C18">
         <v>206830</v>
@@ -3037,7 +3037,7 @@
     </row>
     <row r="19" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C19">
         <v>43.731937030362786</v>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="20" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C20">
         <v>0.2545098725966557</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="21" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C21">
         <v>12862000</v>
@@ -3604,7 +3604,7 @@
     </row>
     <row r="22" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22">
         <v>6387203</v>
@@ -3795,7 +3795,7 @@
     </row>
     <row r="23" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>9.3366427527115707</v>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="24" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C24">
         <v>832</v>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="25" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L25">
         <v>61.538461538500002</v>
@@ -4335,7 +4335,7 @@
     </row>
     <row r="26" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AQ26">
         <v>15.939878725325766</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="27" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C27">
         <v>67.79505520136837</v>
@@ -4552,7 +4552,7 @@
     </row>
     <row r="28" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C28">
         <v>72.707715783022536</v>
@@ -4743,7 +4743,7 @@
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C29">
         <v>70.91</v>
@@ -4934,7 +4934,7 @@
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C30">
         <v>85.93</v>
@@ -5125,7 +5125,7 @@
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C31">
         <v>93.68</v>
@@ -5316,7 +5316,7 @@
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C32">
         <v>13933400</v>
@@ -5507,7 +5507,7 @@
     </row>
     <row r="33" spans="1:66" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C33">
         <v>2181.5</v>
@@ -5698,7 +5698,7 @@
     </row>
     <row r="34" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AF34">
         <v>3.1786330180892608</v>
@@ -5808,7 +5808,7 @@
     </row>
     <row r="35" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AF35">
         <v>37633270846.800255</v>

</xml_diff>

<commit_message>
Johansen test, granger causality for VAR model
</commit_message>
<xml_diff>
--- a/italy_values_dataset.xlsx
+++ b/italy_values_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oldan\Desktop\RuralDevelopment\progetto-tirocinio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686DB74A-80C8-4582-BE44-856648857A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F30E76A-91FA-47AF-93D1-9B8A8208F707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Standard scaling and inverse-transformations on VAR model
Plot needs refining
</commit_message>
<xml_diff>
--- a/italy_values_dataset.xlsx
+++ b/italy_values_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oldan\Desktop\RuralDevelopment\progetto-tirocinio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F30E76A-91FA-47AF-93D1-9B8A8208F707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321C06A8-1BFE-4310-A9C5-CC8CEB63774F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -785,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Refined VAR + added general naive prediction code
</commit_message>
<xml_diff>
--- a/italy_values_dataset.xlsx
+++ b/italy_values_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oldan\Desktop\RuralDevelopment\progetto-tirocinio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321C06A8-1BFE-4310-A9C5-CC8CEB63774F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4D4E64-124A-4AB9-92F5-1E4014AA82F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>